<commit_message>
updated tasks, included KMeans notebook
</commit_message>
<xml_diff>
--- a/resources/Dataset Discovery.xlsx
+++ b/resources/Dataset Discovery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrytirado/git/usc_homework/ML_Project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A550D4-AAEF-8D40-8A12-0585184B255E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEDB5C2-FD4C-404B-82C1-763E2904D495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="520" windowWidth="27180" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="600" windowWidth="27180" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Ideas" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="131">
   <si>
     <t>Dataset</t>
   </si>
@@ -165,24 +165,12 @@
     <t>Test/Train model</t>
   </si>
   <si>
-    <t>RandomForest</t>
-  </si>
-  <si>
     <t>supervised learning in pandas</t>
   </si>
   <si>
-    <t>no StandardScaler, correct?</t>
-  </si>
-  <si>
-    <t>Kmeans</t>
-  </si>
-  <si>
     <t>unsupervised learning in pandas</t>
   </si>
   <si>
-    <t>include StandardScaler, correct?</t>
-  </si>
-  <si>
     <t>Save model</t>
   </si>
   <si>
@@ -201,9 +189,6 @@
     <t>Read tables from PostgresDB to Pandas</t>
   </si>
   <si>
-    <t>Reduce columns, invalid data</t>
-  </si>
-  <si>
     <t>pandas (drop, loc, )</t>
   </si>
   <si>
@@ -213,9 +198,6 @@
     <t>Read model object for validation</t>
   </si>
   <si>
-    <t>Read questions from PostgresDB to app</t>
-  </si>
-  <si>
     <t>Also export StandardScaler object if it was used</t>
   </si>
   <si>
@@ -379,6 +361,63 @@
   </si>
   <si>
     <t>pandas, SqlAlchemy</t>
+  </si>
+  <si>
+    <t>Reduce features, invalid data, age cleanup</t>
+  </si>
+  <si>
+    <t>Get 2 test subjects to take test when ready</t>
+  </si>
+  <si>
+    <t>Validation of model with class users</t>
+  </si>
+  <si>
+    <t>app, HTML page for survey</t>
+  </si>
+  <si>
+    <t>Need working app</t>
+  </si>
+  <si>
+    <t>Stuck  10%</t>
+  </si>
+  <si>
+    <t>Read questions, responses from PostgresDB to app</t>
+  </si>
+  <si>
+    <t>Need images, charts, findings</t>
+  </si>
+  <si>
+    <t>Manually enter questions or code to use DB output</t>
+  </si>
+  <si>
+    <t>have not scaled the data</t>
+  </si>
+  <si>
+    <t>RandomForest classifier,  Scale the data, feature importance</t>
+  </si>
+  <si>
+    <t>Logistic regression, linear regression</t>
+  </si>
+  <si>
+    <t>Kmeans clustering, Scale the data?</t>
+  </si>
+  <si>
+    <t>HTML page for question distribution</t>
+  </si>
+  <si>
+    <t>Tableau table showing tendency to strongly agree/disagrede</t>
+  </si>
+  <si>
+    <t>HTML page for country, age generation</t>
+  </si>
+  <si>
+    <t>More demographics on generation age groups, countries responding</t>
+  </si>
+  <si>
+    <t>Box plot of lapsed time</t>
+  </si>
+  <si>
+    <t>Might tell a story</t>
   </si>
 </sst>
 </file>
@@ -1472,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994141FC-D64F-B24B-87E6-DC040CFE95EB}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,7 +1530,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>38</v>
@@ -1506,31 +1545,31 @@
         <v>41</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1544,10 +1583,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>42</v>
@@ -1557,370 +1596,475 @@
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>48</v>
-      </c>
+      <c r="E7" s="12"/>
       <c r="F7" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E8" s="12"/>
       <c r="F8" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="A10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="16">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>104</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G13" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="A14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>101</v>
-      </c>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="D16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="G16" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>115</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>111</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="16">
+        <v>91</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-    </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G22" s="16">
-        <v>0</v>
+      <c r="G22" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="16">
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="16">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to tasks list
</commit_message>
<xml_diff>
--- a/resources/Dataset Discovery.xlsx
+++ b/resources/Dataset Discovery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrytirado/git/usc_homework/ML_Project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEDB5C2-FD4C-404B-82C1-763E2904D495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F34E9CC-9BF1-D144-88CB-636D8C348D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="600" windowWidth="27180" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="500" windowWidth="27180" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Ideas" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="132">
   <si>
     <t>Dataset</t>
   </si>
@@ -288,9 +288,6 @@
     <t>Henry</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Scott</t>
   </si>
   <si>
@@ -418,6 +415,12 @@
   </si>
   <si>
     <t>Might tell a story</t>
+  </si>
+  <si>
+    <t>Scott, Sushma</t>
+  </si>
+  <si>
+    <t>Team</t>
   </si>
 </sst>
 </file>
@@ -1513,19 +1516,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994141FC-D64F-B24B-87E6-DC040CFE95EB}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1548,7 +1554,7 @@
         <v>72</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1559,7 +1565,7 @@
         <v>64</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>65</v>
@@ -1569,7 +1575,7 @@
         <v>83</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1599,7 +1605,7 @@
         <v>83</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1613,14 +1619,14 @@
         <v>53</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1631,17 +1637,17 @@
         <v>44</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1652,7 +1658,7 @@
         <v>45</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>46</v>
@@ -1662,7 +1668,7 @@
         <v>83</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1673,16 +1679,18 @@
         <v>45</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -1692,19 +1700,19 @@
         <v>45</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1724,7 +1732,7 @@
         <v>57</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G10" s="16">
         <v>0</v>
@@ -1747,7 +1755,7 @@
         <v>55</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>59</v>
@@ -1757,7 +1765,7 @@
         <v>86</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1775,7 +1783,7 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G13" s="16">
         <v>0</v>
@@ -1786,19 +1794,19 @@
         <v>66</v>
       </c>
       <c r="B14" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="16">
         <v>0</v>
@@ -1821,19 +1829,19 @@
         <v>73</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>84</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1841,10 +1849,10 @@
         <v>70</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>84</v>
@@ -1860,15 +1868,15 @@
         <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -1880,17 +1888,17 @@
         <v>74</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1898,17 +1906,17 @@
         <v>70</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>84</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20" s="16">
         <v>0</v>
@@ -1931,19 +1939,19 @@
         <v>68</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1954,13 +1962,13 @@
         <v>69</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>86</v>
@@ -1986,17 +1994,17 @@
         <v>77</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2007,7 +2015,7 @@
         <v>75</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>79</v>
@@ -2016,7 +2024,7 @@
         <v>80</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="G26" s="16">
         <v>0</v>
@@ -2036,7 +2044,7 @@
         <v>78</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>87</v>
@@ -2050,19 +2058,19 @@
         <v>71</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>116</v>
-      </c>
       <c r="F28" s="6" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="G28" s="16">
         <v>0</v>

</xml_diff>